<commit_message>
R scripts and data files
</commit_message>
<xml_diff>
--- a/KevinData20170202/CODE BOOK FOR ALL THE CENSUS VARIABLES I PULLED.xlsx
+++ b/KevinData20170202/CODE BOOK FOR ALL THE CENSUS VARIABLES I PULLED.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\700\700 project\all data sets for analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\MsseProject\KevinData20170202\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26190" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26196" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="141">
   <si>
     <t>AGE030200D</t>
   </si>
@@ -339,6 +339,114 @@
   </si>
   <si>
     <t>Supplemental medical insurance (Medicare) - total persons enrolled July 1, 2000</t>
+  </si>
+  <si>
+    <t>populationApril2000</t>
+  </si>
+  <si>
+    <t>populationJuly2000</t>
+  </si>
+  <si>
+    <t>populationMedianAgeApril2000</t>
+  </si>
+  <si>
+    <t>bankOfficesJune2000</t>
+  </si>
+  <si>
+    <t>bankDepositsJune2000</t>
+  </si>
+  <si>
+    <t>unemployment</t>
+  </si>
+  <si>
+    <t>unemploymentRate</t>
+  </si>
+  <si>
+    <t>violentCrimes</t>
+  </si>
+  <si>
+    <t>educationHighSchoolOrAboveRate</t>
+  </si>
+  <si>
+    <t>insuranceOrMedicare</t>
+  </si>
+  <si>
+    <t>medicare</t>
+  </si>
+  <si>
+    <t>householdsMaleNoWife</t>
+  </si>
+  <si>
+    <t>householdsFemaleNoHusband</t>
+  </si>
+  <si>
+    <t>ownerOccupiedHomesHouseholderBlackOrAfricanAmerican</t>
+  </si>
+  <si>
+    <t>ownerOccupiedHomesHouseholderHispanicOrLatino</t>
+  </si>
+  <si>
+    <t>sampleMedianHousingUnitValue</t>
+  </si>
+  <si>
+    <t>renterOccupiedHousingUnits</t>
+  </si>
+  <si>
+    <t>renterOccupiedHomesHouseholderBlackOrAfricanAmerican</t>
+  </si>
+  <si>
+    <t>renterOccupiedHomesHouseholderHispanicOrLatino</t>
+  </si>
+  <si>
+    <t>perCapitaIncome</t>
+  </si>
+  <si>
+    <t>meanHouseholdEarnings</t>
+  </si>
+  <si>
+    <t>householdsWithSocialSecurityIncome</t>
+  </si>
+  <si>
+    <t>medianHouseholdIncome2000</t>
+  </si>
+  <si>
+    <t>medianHouseholdIncome1999</t>
+  </si>
+  <si>
+    <t>peopleInPovertyRate</t>
+  </si>
+  <si>
+    <t>landArea</t>
+  </si>
+  <si>
+    <t>perCapitaPersonalIncome</t>
+  </si>
+  <si>
+    <t>populationPerSquareMile</t>
+  </si>
+  <si>
+    <t>urbanPopulationSample</t>
+  </si>
+  <si>
+    <t>malePopulationCompleteCount</t>
+  </si>
+  <si>
+    <t>femalePopulationCompleteCount</t>
+  </si>
+  <si>
+    <t>populationOfOneRaceWhiteAloneCompleteCount</t>
+  </si>
+  <si>
+    <t>populationOfOneRaceBlackOrAfricanAmericanAloneCompleteCount</t>
+  </si>
+  <si>
+    <t>populationBelowPovertyLevel</t>
+  </si>
+  <si>
+    <t>socialSecurityBenefitRecipients</t>
+  </si>
+  <si>
+    <t>supplementalSecurityIncomeRecipients</t>
   </si>
 </sst>
 </file>
@@ -656,793 +764,1047 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="124" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="124" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE("independent &lt;- renameColumn(independent, """, A2, """, """, B2, """)")</f>
+        <v>independent &lt;- renameColumn(independent, "AGE030200D", "populationApril2000")</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
         <v>281424602</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C52" si="0">CONCATENATE("independent &lt;- renameColumn(independent, """, A3, """, """, B3, """)")</f>
+        <v>independent &lt;- renameColumn(independent, "AGE040200D", "populationJuly2000")</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
         <v>282171957</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "AGE050200D", "populationMedianAgeApril2000")</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>35.299999999999997</v>
       </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "BNK010200D", "bankOfficesJune2000")</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7">
         <v>84848</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "BNK050200D", "bankDepositsJune2000")</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9">
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9">
         <v>3966224000</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "CLF030200D", "unemployment")</v>
+      </c>
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11">
         <v>5692000</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
       <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "CLF040200D", "unemploymentRate")</v>
+      </c>
+      <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>4</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "CRM110200D", "violentCrimes")</v>
+      </c>
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14">
         <v>1349339</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>94</v>
       </c>
       <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "EDU635200D", "educationHighSchoolOrAboveRate")</v>
+      </c>
+      <c r="D16" t="s">
         <v>95</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>80.400000000000006</v>
       </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HEA010200D", "insuranceOrMedicare")</v>
+      </c>
+      <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18">
         <v>38761628</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>103</v>
       </c>
       <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HEA070200D", "medicare")</v>
+      </c>
+      <c r="D19" t="s">
         <v>104</v>
       </c>
-      <c r="C19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19">
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19">
         <v>36908539</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
       <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HSD150200D", "householdsMaleNoWife")</v>
+      </c>
+      <c r="D20" t="s">
         <v>40</v>
       </c>
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20">
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20">
         <v>4394012</v>
       </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HSD170200D", "householdsFemaleNoHusband")</v>
+      </c>
+      <c r="D21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21">
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21">
         <v>12900103</v>
       </c>
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
       <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HSG455200D", "ownerOccupiedHomesHouseholderBlackOrAfricanAmerican")</v>
+      </c>
+      <c r="D23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23">
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23">
         <v>5577734</v>
       </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
       <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HSG460200D", "ownerOccupiedHomesHouseholderHispanicOrLatino")</v>
+      </c>
+      <c r="D24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24">
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24">
         <v>4212520</v>
       </c>
-      <c r="F24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>45</v>
       </c>
       <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HSG495200D", "sampleMedianHousingUnitValue")</v>
+      </c>
+      <c r="D25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>47</v>
       </c>
-      <c r="D25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25">
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25">
         <v>119600</v>
       </c>
-      <c r="F25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
       <c r="B26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HSG680200D", "renterOccupiedHousingUnits")</v>
+      </c>
+      <c r="D26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26">
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26">
         <v>35664348</v>
       </c>
-      <c r="F26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
       <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HSG695200D", "renterOccupiedHomesHouseholderBlackOrAfricanAmerican")</v>
+      </c>
+      <c r="D27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27">
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27">
         <v>6477348</v>
       </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>52</v>
       </c>
       <c r="B28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "HSG700200D", "renterOccupiedHomesHouseholderHispanicOrLatino")</v>
+      </c>
+      <c r="D28" t="s">
         <v>53</v>
       </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28">
         <v>5009882</v>
       </c>
-      <c r="F28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>54</v>
       </c>
       <c r="B30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "INC110199D", "medianHouseholdIncome1999")</v>
+      </c>
+      <c r="D30" t="s">
         <v>55</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>47</v>
       </c>
-      <c r="D30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30">
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30">
         <v>41994</v>
       </c>
-      <c r="F30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
       <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "INC415199D", "meanHouseholdEarnings")</v>
+      </c>
+      <c r="D31" t="s">
         <v>57</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>47</v>
       </c>
-      <c r="D31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31">
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31">
         <v>56604</v>
       </c>
-      <c r="F31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>58</v>
       </c>
       <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "INC420200D", "householdsWithSocialSecurityIncome")</v>
+      </c>
+      <c r="D32" t="s">
         <v>59</v>
       </c>
-      <c r="C32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32">
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32">
         <v>27084417</v>
       </c>
-      <c r="F32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>60</v>
       </c>
       <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "INC910199D", "perCapitaIncome")</v>
+      </c>
+      <c r="D33" t="s">
         <v>61</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>47</v>
       </c>
-      <c r="D33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33">
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33">
         <v>21587</v>
       </c>
-      <c r="F33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>62</v>
       </c>
       <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "IPE010200D", "medianHouseholdIncome2000")</v>
+      </c>
+      <c r="D35" t="s">
         <v>63</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
         <v>47</v>
       </c>
-      <c r="D35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35">
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35">
         <v>41990</v>
       </c>
-      <c r="F35" t="s">
+      <c r="H35" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>65</v>
       </c>
       <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "IPE120200D", "peopleInPovertyRate")</v>
+      </c>
+      <c r="D36" t="s">
         <v>66</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>67</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
         <v>10</v>
       </c>
-      <c r="E36">
+      <c r="G36">
         <v>11.3</v>
       </c>
-      <c r="F36" t="s">
+      <c r="H36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>68</v>
       </c>
       <c r="B38" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "LND110200D", "landArea")</v>
+      </c>
+      <c r="D38" t="s">
         <v>69</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>70</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F38" t="s">
         <v>71</v>
       </c>
-      <c r="E38">
+      <c r="G38">
         <v>3537438.44</v>
       </c>
-      <c r="F38" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
       <c r="B40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "PIN020200D", "perCapitaPersonalIncome")</v>
+      </c>
+      <c r="D40" t="s">
         <v>73</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>47</v>
       </c>
-      <c r="D40" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40">
+      <c r="F40" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40">
         <v>29847</v>
       </c>
-      <c r="F40" t="s">
+      <c r="H40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>75</v>
       </c>
       <c r="B42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "POP060200D", "populationPerSquareMile")</v>
+      </c>
+      <c r="D42" t="s">
         <v>76</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
         <v>30</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F42" t="s">
         <v>10</v>
       </c>
-      <c r="E42">
+      <c r="G42">
         <v>79.599999999999994</v>
       </c>
-      <c r="F42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>77</v>
       </c>
       <c r="B43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "POP110200D", "urbanPopulationSample")</v>
+      </c>
+      <c r="D43" t="s">
         <v>78</v>
       </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43">
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43">
         <v>222358309</v>
       </c>
-      <c r="F43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>79</v>
       </c>
       <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "POP150200D", "malePopulationCompleteCount")</v>
+      </c>
+      <c r="D44" t="s">
         <v>80</v>
       </c>
-      <c r="C44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44">
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44">
         <v>138053563</v>
       </c>
-      <c r="F44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>81</v>
       </c>
       <c r="B45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "POP160200D", "femalePopulationCompleteCount")</v>
+      </c>
+      <c r="D45" t="s">
         <v>82</v>
       </c>
-      <c r="C45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45">
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45">
         <v>143368343</v>
       </c>
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>83</v>
       </c>
       <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "POP220200D", "populationOfOneRaceWhiteAloneCompleteCount")</v>
+      </c>
+      <c r="D46" t="s">
         <v>84</v>
       </c>
-      <c r="C46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46">
+      <c r="E46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46">
         <v>211460626</v>
       </c>
-      <c r="F46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>85</v>
       </c>
       <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "POP250200D", "populationOfOneRaceBlackOrAfricanAmericanAloneCompleteCount")</v>
+      </c>
+      <c r="D47" t="s">
         <v>86</v>
       </c>
-      <c r="C47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D47" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47">
+      <c r="E47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47">
         <v>34658190</v>
       </c>
-      <c r="F47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>87</v>
       </c>
       <c r="B49" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "PVY020199D", "populationBelowPovertyLevel")</v>
+      </c>
+      <c r="D49" t="s">
         <v>88</v>
       </c>
-      <c r="C49" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49">
+      <c r="E49" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49">
         <v>33899812</v>
       </c>
-      <c r="F49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>89</v>
       </c>
       <c r="B51" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "SPR010200D", "socialSecurityBenefitRecipients")</v>
+      </c>
+      <c r="D51" t="s">
         <v>90</v>
       </c>
-      <c r="C51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51">
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51">
         <v>44314807</v>
       </c>
-      <c r="F51" t="s">
+      <c r="H51" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>92</v>
       </c>
       <c r="B52" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>independent &lt;- renameColumn(independent, "SPR410200D", "supplementalSecurityIncomeRecipients")</v>
+      </c>
+      <c r="D52" t="s">
         <v>93</v>
       </c>
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E52">
+      <c r="E52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52">
         <v>6601009</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>96</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>101</v>
       </c>

</xml_diff>